<commit_message>
add relation values to input for SNG from biogas
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methane/Model_Data_Base_methane_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methane/Model_Data_Base_methane_4_InOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2758BBB-464F-4578-B390-0C66FEF0F83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E80F7D-C7BD-4A52-82DB-1249CC81A3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
   <si>
     <t>Unit</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Digester</t>
   </si>
   <si>
-    <t>CO2_MethaneMix</t>
-  </si>
-  <si>
     <t>Methanation</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>co2</t>
-  </si>
-  <si>
     <t>start_up_cost</t>
   </si>
   <si>
@@ -335,12 +329,6 @@
   </si>
   <si>
     <t>Auxilliary</t>
-  </si>
-  <si>
-    <t>heat_high</t>
-  </si>
-  <si>
-    <t>internal_heat</t>
   </si>
   <si>
     <t>heat_low</t>
@@ -557,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5CD33EB7-C7FA-420A-B41D-54E455F2582D}" name="Table17" displayName="Table17" ref="A1:Q10" totalsRowShown="0">
-  <autoFilter ref="A1:Q10" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5CD33EB7-C7FA-420A-B41D-54E455F2582D}" name="Table17" displayName="Table17" ref="A1:Q8" totalsRowShown="0">
+  <autoFilter ref="A1:Q8" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{8642BBE5-9C8A-4B22-9A88-832555EF4D56}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{ED663D39-C262-40E4-93B2-16669EE6A517}" name="Object_type"/>
@@ -965,7 +953,7 @@
         <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>34</v>
@@ -974,22 +962,22 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L1" t="s">
         <v>35</v>
@@ -1001,7 +989,7 @@
         <v>25</v>
       </c>
       <c r="O1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P1" t="s">
         <v>36</v>
@@ -1010,57 +998,57 @@
         <v>37</v>
       </c>
       <c r="R1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>0.75</v>
@@ -1076,13 +1064,13 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
@@ -1090,13 +1078,13 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
@@ -1106,13 +1094,13 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1121,13 +1109,13 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N9" s="5">
         <v>1.4865951742627345E-3</v>
@@ -1137,13 +1125,13 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1164,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A86F1AE-0A9A-41EF-AAC6-2EFA35CD0F28}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1177,7 +1165,7 @@
     <col min="3" max="17" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1191,10 +1179,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1203,84 +1191,84 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N1" t="s">
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
       <c r="G4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K5">
         <v>5.8500000000000002E-3</v>
@@ -1289,106 +1277,71 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>85</v>
+      </c>
+      <c r="K6">
+        <v>0.86792452830188682</v>
+      </c>
+      <c r="L6">
+        <v>46</v>
+      </c>
+      <c r="N6">
+        <v>0.5168539325842697</v>
+      </c>
+      <c r="O6">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" t="s">
-        <v>89</v>
-      </c>
-      <c r="O8">
-        <v>0.4</v>
-      </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8" xr:uid="{FB6665C5-F838-40AC-919C-58EE6E1C9E29}">
-      <formula1>"h, D, W, M, Q, Y"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1504,33 +1457,33 @@
         <v>33</v>
       </c>
       <c r="Z1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1563,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -1571,25 +1524,25 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1619,7 +1572,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="Z3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -1627,42 +1580,42 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1680,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1743,15 +1696,15 @@
         <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1766,7 +1719,7 @@
         <v>4.147E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1774,10 +1727,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1786,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1826,7 +1779,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
@@ -1836,17 +1789,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
@@ -1856,37 +1809,37 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
@@ -1896,17 +1849,17 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>